<commit_message>
second circle is doing. use data of ZL, RF KNN SVR not done.
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MLDesignAl\TheFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C60415-B911-4944-861D-6C4F15246CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F56AC48-C1D9-4AF0-8F78-89438BD9D8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33240" yWindow="3075" windowWidth="22140" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36405" yWindow="2295" windowWidth="19320" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>成分-UTS（所有可用数据）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +64,10 @@
   </si>
   <si>
     <t>MAPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成分-UTS（铸铝）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -112,10 +116,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -398,22 +402,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -423,76 +427,147 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.6472</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.1865</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.70660000000000001</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.15959999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.51580000000000004</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.16589999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.64259999999999995</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.18060000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.69820000000000004</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.13730000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.74329999999999996</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>0.15529999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.2029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.71550000000000002</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>0.16450000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.74329999999999996</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.15529999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>0.72260000000000002</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.15579999999999999</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.71550000000000002</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.16450000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.72260000000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.15579999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
next step to do the SVR model which use the data of ElementTreatment-EL. Details read "summary"
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MLDesignAl\TheFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7F0AD9-9C7B-4ABA-98E6-20DD88136079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B47FB7-C32D-47A2-AB4F-44D1659F25D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37500" yWindow="2565" windowWidth="19320" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35580" yWindow="1635" windowWidth="19320" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
-  <si>
-    <t>成分-UTS（所有可用数据）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="20">
   <si>
     <t>模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +72,38 @@
   </si>
   <si>
     <t>成分工艺-UTS（所有）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成分El-UTS（所有）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成分工艺El-UTS（所有）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XGB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LGBM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成分-UTS（所有可用数据，部分元素）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成分-UTS（所有可用数据，全部元素）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成分-EL（所有可用数据，全部元素）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成分工艺-EL（所有）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -83,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +124,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -122,10 +157,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,14 +171,18 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,40 +461,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>0.6472</v>
@@ -461,23 +506,23 @@
         <v>0.1865</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>0.70660000000000001</v>
@@ -486,7 +531,7 @@
         <v>0.15959999999999999</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
         <v>0.51580000000000004</v>
@@ -495,23 +540,23 @@
         <v>0.16589999999999999</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>0.64259999999999995</v>
@@ -519,8 +564,8 @@
       <c r="C5" s="2">
         <v>0.18060000000000001</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="E5" s="2">
         <v>0.69820000000000004</v>
@@ -529,23 +574,28 @@
         <v>0.13730000000000001</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
+      <c r="M5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>0.74329999999999996</v>
@@ -554,7 +604,7 @@
         <v>0.15529999999999999</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2">
         <v>0.19689999999999999</v>
@@ -562,8 +612,8 @@
       <c r="F6" s="2">
         <v>0.2029</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>3</v>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="H6" s="2">
         <v>0.69410000000000005</v>
@@ -572,14 +622,28 @@
         <v>0.16189999999999999</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
+      <c r="M6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>0.71550000000000002</v>
@@ -587,8 +651,8 @@
       <c r="C7" s="2">
         <v>0.16450000000000001</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E7" s="2">
         <v>0.64480000000000004</v>
@@ -597,12 +661,12 @@
         <v>0.1472</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="4" t="s">
-        <v>3</v>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="K7" s="2">
         <v>0.69169999999999998</v>
@@ -610,10 +674,24 @@
       <c r="L7" s="2">
         <v>0.12959999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="M7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>0.72260000000000002</v>
@@ -621,8 +699,8 @@
       <c r="C8" s="2">
         <v>0.15579999999999999</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="E8" s="2">
         <v>0.64849999999999997</v>
@@ -630,8 +708,8 @@
       <c r="F8" s="2">
         <v>0.15160000000000001</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>5</v>
+      <c r="G8" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="H8" s="2">
         <v>0.72699999999999998</v>
@@ -640,14 +718,33 @@
         <v>0.15529999999999999</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="4" t="s">
-        <v>7</v>
+      <c r="M8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.1467</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E9" s="2">
         <v>0.68830000000000002</v>
@@ -655,8 +752,8 @@
       <c r="F9" s="2">
         <v>0.13769999999999999</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>6</v>
+      <c r="G9" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="H9" s="2">
         <v>0.71460000000000001</v>
@@ -664,8 +761,8 @@
       <c r="I9" s="2">
         <v>0.16039999999999999</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>5</v>
+      <c r="J9" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K9" s="2">
         <v>0.8397</v>
@@ -673,10 +770,33 @@
       <c r="L9" s="2">
         <v>9.74E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G10" s="4" t="s">
-        <v>7</v>
+      <c r="M9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0.74339999999999995</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.12230000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.73509999999999998</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.15970000000000001</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H10" s="2">
         <v>0.71779999999999999</v>
@@ -684,8 +804,8 @@
       <c r="I10" s="2">
         <v>0.15479999999999999</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>6</v>
+      <c r="J10" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="K10" s="2">
         <v>0.80569999999999997</v>
@@ -693,10 +813,33 @@
       <c r="L10" s="2">
         <v>0.1012</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J11" s="4" t="s">
-        <v>7</v>
+      <c r="M10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.77349999999999997</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.13220000000000001</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.73549999999999993</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="K11" s="2">
         <v>0.82469999999999999</v>
@@ -704,13 +847,265 @@
       <c r="L11" s="2">
         <v>9.9900000000000003E-2</v>
       </c>
+      <c r="M11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.72909999999999997</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.14419999999999999</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0.89949999999999997</v>
+      </c>
+      <c r="R11" s="2">
+        <v>8.7099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.80249999999999999</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.1217</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0.86619999999999997</v>
+      </c>
+      <c r="R12" s="2">
+        <v>9.0800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="P13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0.88239999999999996</v>
+      </c>
+      <c r="R13" s="2">
+        <v>8.8800000000000004E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0.92330000000000001</v>
+      </c>
+      <c r="R14" s="2">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>8.09E-2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.55149999999999999</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0.91480000000000006</v>
+      </c>
+      <c r="R15" s="2">
+        <v>7.9199999999999993E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>-0.50860000000000005</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.45879999999999999</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.21510000000000001</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.34210000000000002</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.45660000000000001</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.317</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.33789999999999998</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.28170000000000001</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>-0.41770000000000002</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.47560000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.31819999999999998</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.29189999999999999</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.42520000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.4647</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.30549999999999999</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.6905</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.37390000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.44840000000000002</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.28710000000000002</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.57430000000000003</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="P6:R6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M5:O5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>